<commit_message>
Added pull-up resistor to NRST line, changed I2C and PWM functions mapping
</commit_message>
<xml_diff>
--- a/BOM FreeJoy Controller Lite.xlsx
+++ b/BOM FreeJoy Controller Lite.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YandexDisk\Projects Altium\FreeJoy\FreeJoy Controller Lite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YandexDisk\Projects\FreeJoy\FreeJoy Controller Lite\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -50,7 +50,16 @@
     <t>4.7nF 250V</t>
   </si>
   <si>
-    <t>C2, C3, C11</t>
+    <t>C2, C5, C6, C7, C8, C9, C12</t>
+  </si>
+  <si>
+    <t>0.1uF ± 10%, 25V, X7R, SMD 0603</t>
+  </si>
+  <si>
+    <t>100nF</t>
+  </si>
+  <si>
+    <t>C3, C4, C11</t>
   </si>
   <si>
     <t>1uF ± 10%, 16V, X7R, SMD 0603</t>
@@ -59,15 +68,6 @@
     <t>1uF</t>
   </si>
   <si>
-    <t>C4, C5, C6, C7, C8, C12, C15</t>
-  </si>
-  <si>
-    <t>0.1uF ± 10%, 25V, X7R, SMD 0603</t>
-  </si>
-  <si>
-    <t>100nF</t>
-  </si>
-  <si>
     <t>C10, C13, C14</t>
   </si>
   <si>
@@ -158,7 +158,7 @@
     <t>27R</t>
   </si>
   <si>
-    <t>R5, R9, R10</t>
+    <t>R5, R6, R10, R11</t>
   </si>
   <si>
     <t>4K7 ± 1%, SMD 0603</t>
@@ -167,7 +167,7 @@
     <t>4K7</t>
   </si>
   <si>
-    <t>R6, R7</t>
+    <t>R7, R8</t>
   </si>
   <si>
     <t>470R ± 1%, SMD 0603</t>
@@ -176,7 +176,7 @@
     <t>470R</t>
   </si>
   <si>
-    <t>R8</t>
+    <t>R9</t>
   </si>
   <si>
     <t>1K ± 1%, SMD 0603</t>
@@ -206,21 +206,21 @@
     <t>XP2</t>
   </si>
   <si>
+    <t>PLS-5</t>
+  </si>
+  <si>
+    <t>PROG</t>
+  </si>
+  <si>
+    <t>XP3</t>
+  </si>
+  <si>
     <t>PLD-4</t>
   </si>
   <si>
     <t>BOOT</t>
   </si>
   <si>
-    <t>XP3</t>
-  </si>
-  <si>
-    <t>PLS-5</t>
-  </si>
-  <si>
-    <t>PROG</t>
-  </si>
-  <si>
     <t>XP4</t>
   </si>
   <si>
@@ -251,25 +251,25 @@
     <t>XP8</t>
   </si>
   <si>
+    <t>AXIS-A4</t>
+  </si>
+  <si>
+    <t>XP9</t>
+  </si>
+  <si>
     <t>SPI/A5</t>
   </si>
   <si>
-    <t>XP9</t>
+    <t>XP10</t>
   </si>
   <si>
     <t>SPI/A6</t>
   </si>
   <si>
-    <t>XP10</t>
+    <t>XP11</t>
   </si>
   <si>
     <t>SHIFT REG/A7</t>
-  </si>
-  <si>
-    <t>XP11</t>
-  </si>
-  <si>
-    <t>AXIS-A4</t>
   </si>
   <si>
     <t>XP12</t>
@@ -698,7 +698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -709,10 +709,10 @@
         <v>9</v>
       </c>
       <c r="D3" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -723,7 +723,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="4">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -877,7 +877,7 @@
         <v>45</v>
       </c>
       <c r="D15" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>